<commit_message>
MODIFY: arrangement of sections and notes
</commit_message>
<xml_diff>
--- a/machine_learning_concepts.xlsx
+++ b/machine_learning_concepts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandy Lauguico\Documents\01-learn-in-public\product\r-linear-regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1543575-3D0A-4A75-8A07-05D96D625808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733131F5-4BD0-4643-A454-B2FBCA5BF8C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{06EE85D0-79E0-4C85-BDA9-B6537CCBBDD5}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{06EE85D0-79E0-4C85-BDA9-B6537CCBBDD5}"/>
   </bookViews>
   <sheets>
     <sheet name="What is Machine Learning" sheetId="1" r:id="rId1"/>
@@ -1278,17 +1278,12 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1303,10 +1298,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1314,7 +1315,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -13983,8 +13983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3ABF26F-C6E8-4827-BF65-41F0D0CD8A51}">
   <dimension ref="A1:U63"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="H25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14015,29 +14015,29 @@
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="G2" s="47" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="G2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="47"/>
-      <c r="J2" s="46" t="s">
+      <c r="H2" s="54"/>
+      <c r="J2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="M2" s="46" t="s">
+      <c r="K2" s="53"/>
+      <c r="M2" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
@@ -14058,18 +14058,18 @@
       <c r="H3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="55" t="s">
         <v>266</v>
       </c>
-      <c r="K3" s="48"/>
-      <c r="N3" s="48" t="s">
+      <c r="K3" s="55"/>
+      <c r="N3" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
@@ -14113,18 +14113,18 @@
         <f>IF(G5 &gt;= $D$8, $E$8, IF(AND(G5 &lt; $D$8, G5 &gt;= $D$7), $E$7, IF(AND(G5 &lt; $D$7, G5 &gt;= $D$6), $E$6, IF(AND(G5 &lt; $D$6, G5 &gt;= $D$5), $E$5, IF(AND(G5 &lt; $D$5, G5 &gt;= $D$4), $E$4, "Upskill ka muna")))))</f>
         <v>40000</v>
       </c>
-      <c r="J5" s="49" t="s">
+      <c r="J5" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="49"/>
-      <c r="N5" s="51" t="s">
+      <c r="K5" s="56"/>
+      <c r="N5" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="53"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="52"/>
       <c r="T5" s="19"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
@@ -14144,14 +14144,14 @@
         <f t="shared" ref="H6:H16" si="0">IF(G6 &gt;= $D$8, $E$8, IF(AND(G6 &lt; $D$8, G6 &gt;= $D$7), $E$7, IF(AND(G6 &lt; $D$7, G6 &gt;= $D$6), $E$6, IF(AND(G6 &lt; $D$6, G6 &gt;= $D$5), $E$5, IF(AND(G6 &lt; $D$5, G6 &gt;= $D$4), $E$4, "Upskill ka muna")))))</f>
         <v>40000</v>
       </c>
-      <c r="N6" s="50" t="s">
+      <c r="N6" s="49" t="s">
         <v>270</v>
       </c>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
-      <c r="Q6" s="50"/>
-      <c r="R6" s="50"/>
-      <c r="S6" s="50"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
       <c r="T6" s="19"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
@@ -14171,18 +14171,18 @@
         <f t="shared" si="0"/>
         <v>80000</v>
       </c>
-      <c r="J7" s="47" t="s">
+      <c r="J7" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="N7" s="50" t="s">
+      <c r="K7" s="54"/>
+      <c r="N7" s="49" t="s">
         <v>271</v>
       </c>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="50"/>
-      <c r="S7" s="50"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
       <c r="T7" s="19"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
@@ -14208,14 +14208,14 @@
       <c r="K8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="50" t="s">
+      <c r="N8" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
       <c r="T8" s="19"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
@@ -14232,14 +14232,14 @@
       <c r="K9" s="14">
         <v>40000</v>
       </c>
-      <c r="N9" s="51" t="s">
+      <c r="N9" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="53"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="52"/>
       <c r="T9" s="19"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
@@ -14256,14 +14256,14 @@
       <c r="K10" s="4">
         <v>60000</v>
       </c>
-      <c r="N10" s="51" t="s">
+      <c r="N10" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="53"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="52"/>
       <c r="T10" s="19"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
@@ -14295,14 +14295,14 @@
       <c r="K12" s="4">
         <v>100000</v>
       </c>
-      <c r="N12" s="54" t="s">
+      <c r="N12" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="54"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="54"/>
-      <c r="S12" s="54"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="G13" s="4">
@@ -14442,10 +14442,10 @@
       </c>
     </row>
     <row r="22" spans="7:15" x14ac:dyDescent="0.35">
-      <c r="J22" s="54" t="s">
+      <c r="J22" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="K22" s="54"/>
+      <c r="K22" s="47"/>
     </row>
     <row r="23" spans="7:15" x14ac:dyDescent="0.35">
       <c r="N23" t="s">
@@ -14520,10 +14520,10 @@
       </c>
     </row>
     <row r="39" spans="10:15" x14ac:dyDescent="0.35">
-      <c r="N39" s="55" t="s">
+      <c r="N39" s="48" t="s">
         <v>272</v>
       </c>
-      <c r="O39" s="55"/>
+      <c r="O39" s="48"/>
     </row>
     <row r="40" spans="10:15" x14ac:dyDescent="0.35">
       <c r="N40" s="18" t="s">
@@ -14550,7 +14550,7 @@
         <v>2</v>
       </c>
       <c r="O42" s="4">
-        <f t="shared" ref="O41:O60" si="1">20000*(N42)+20000</f>
+        <f t="shared" ref="O42:O60" si="1">20000*(N42)+20000</f>
         <v>60000</v>
       </c>
     </row>
@@ -14729,25 +14729,18 @@
       </c>
     </row>
     <row r="63" spans="10:20" x14ac:dyDescent="0.35">
-      <c r="N63" s="54" t="s">
+      <c r="N63" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="O63" s="54"/>
-      <c r="P63" s="54"/>
-      <c r="Q63" s="54"/>
+      <c r="O63" s="47"/>
+      <c r="P63" s="47"/>
+      <c r="Q63" s="47"/>
       <c r="R63" s="8"/>
       <c r="S63" s="8"/>
       <c r="T63" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="N63:Q63"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="N12:S12"/>
-    <mergeCell ref="N8:S8"/>
-    <mergeCell ref="N9:S9"/>
-    <mergeCell ref="N10:S10"/>
     <mergeCell ref="M2:T2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
@@ -14759,6 +14752,13 @@
     <mergeCell ref="N6:S6"/>
     <mergeCell ref="N7:S7"/>
     <mergeCell ref="N5:S5"/>
+    <mergeCell ref="N63:Q63"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="N12:S12"/>
+    <mergeCell ref="N8:S8"/>
+    <mergeCell ref="N9:S9"/>
+    <mergeCell ref="N10:S10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14769,7 +14769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F11F37-6F43-47A3-ACEA-6A0ABD34840B}">
   <dimension ref="B1:T11"/>
   <sheetViews>
-    <sheetView topLeftCell="G31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
@@ -17923,44 +17923,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="53" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="I1" s="56" t="s">
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="I1" s="57" t="s">
         <v>245</v>
       </c>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="Q1" s="56" t="s">
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="Q1" s="57" t="s">
         <v>240</v>
       </c>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="X1" s="56" t="s">
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="X1" s="57" t="s">
         <v>246</v>
       </c>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="56"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="Y3" s="38" t="s">
@@ -19261,8 +19261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C23027-444A-4A5F-989F-F5E5429A7DF6}">
   <dimension ref="A1:AV347"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AZ6" sqref="AZ6"/>
+    <sheetView tabSelected="1" topLeftCell="AA25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AR44" sqref="AR44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19284,58 +19284,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="N1" s="46" t="s">
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="N1" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="U1" s="46" t="s">
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="U1" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AC1" s="46" t="s">
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AC1" s="53" t="s">
         <v>175</v>
       </c>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AN1" s="57" t="s">
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="53"/>
+      <c r="AL1" s="53"/>
+      <c r="AN1" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="AO1" s="57"/>
-      <c r="AP1" s="57"/>
-      <c r="AQ1" s="57"/>
-      <c r="AR1" s="57"/>
-      <c r="AS1" s="57"/>
-      <c r="AT1" s="57"/>
-      <c r="AU1" s="57"/>
+      <c r="AO1" s="58"/>
+      <c r="AP1" s="58"/>
+      <c r="AQ1" s="58"/>
+      <c r="AR1" s="58"/>
+      <c r="AS1" s="58"/>
+      <c r="AT1" s="58"/>
+      <c r="AU1" s="58"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.35">
       <c r="O2" t="s">
@@ -21187,7 +21187,7 @@
       <c r="X88" t="s">
         <v>107</v>
       </c>
-      <c r="Y88" s="58">
+      <c r="Y88" s="46">
         <f>R202</f>
         <v>1255838122</v>
       </c>
@@ -23153,7 +23153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395E558A-FB4C-4273-8454-8ABD44ECE433}">
   <dimension ref="I1:V658"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
@@ -45134,7 +45134,7 @@
   <dimension ref="B2:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>